<commit_message>
shuffled files around for cleaner organization
</commit_message>
<xml_diff>
--- a/scan_cards_pinout.xlsx
+++ b/scan_cards_pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_works\dev\HomeAutomation\Projects\KeithleyScanCard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_works\dev\test\GH1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBF87F1-8623-4DCA-999D-5012417564BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B96AFC-309D-4879-BAE8-C95FD29F0D68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="1320" windowWidth="33510" windowHeight="17790" xr2:uid="{156A2997-E9DE-4EA5-8776-7E927FE535DA}"/>
+    <workbookView xWindow="2535" yWindow="0" windowWidth="36675" windowHeight="21600" xr2:uid="{156A2997-E9DE-4EA5-8776-7E927FE535DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="27">
   <si>
     <t>GND</t>
   </si>
@@ -78,18 +78,6 @@
     <t>SCL</t>
   </si>
   <si>
-    <t>mavi beyaz</t>
-  </si>
-  <si>
-    <t>yesil beyaz</t>
-  </si>
-  <si>
-    <t>kahve beyaz</t>
-  </si>
-  <si>
-    <t>turuncu beyaz</t>
-  </si>
-  <si>
     <t>Header Pin #</t>
   </si>
   <si>
@@ -99,16 +87,31 @@
     <t>Note: keithley numbers pins sequentially one row and moves on on the other row. Eagle uses row1, row2, row1, row2 order.</t>
   </si>
   <si>
-    <t>mavi</t>
-  </si>
-  <si>
-    <t>kahve</t>
-  </si>
-  <si>
-    <t>turuncu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yesil </t>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>blue/white</t>
+  </si>
+  <si>
+    <t>brown/white</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>orange/white</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>green/white</t>
+  </si>
+  <si>
+    <t>wire</t>
   </si>
 </sst>
 </file>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1A0BD1-587A-4C62-BF6D-3F9061440700}">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,17 +519,18 @@
     <col min="6" max="6" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="18" width="9.140625" style="2"/>
+    <col min="10" max="10" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="9.140625" style="2"/>
     <col min="19" max="19" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -546,8 +550,11 @@
       <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -566,11 +573,11 @@
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -592,11 +599,11 @@
       <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -616,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -638,11 +645,11 @@
       <c r="H5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -662,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -684,11 +691,11 @@
       <c r="H7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -708,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -730,11 +737,11 @@
       <c r="H9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -754,7 +761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -773,11 +780,11 @@
       <c r="H11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="S11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -797,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -817,7 +824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -840,11 +847,11 @@
       <c r="H14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S14" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -864,7 +871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -884,7 +891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -906,7 +913,7 @@
       </c>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -926,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -949,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -969,7 +976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -992,7 +999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1012,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1035,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1055,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1078,7 +1085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1118,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1138,7 +1145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1158,7 +1165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1181,11 +1188,11 @@
       <c r="H30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S30" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J30" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1249,7 +1256,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>